<commit_message>
Plan de capacitacion actualizado
</commit_message>
<xml_diff>
--- a/private/Documentación/Plan de Capacitacion/Plan de capacitación.xlsx
+++ b/private/Documentación/Plan de Capacitacion/Plan de capacitación.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itzman\Documents\ADMIN_ID+1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Itzman\Documents\ADMIN_ID+1\Plan de Capacitacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t xml:space="preserve">Descripción </t>
   </si>
@@ -35,43 +35,46 @@
     <t xml:space="preserve"> Topico</t>
   </si>
   <si>
-    <t xml:space="preserve">Registro </t>
-  </si>
-  <si>
     <t>30 min.</t>
   </si>
   <si>
-    <t>Completar el llenado de los campos para poder tener una validacion de los datos del alumno o profesor.</t>
-  </si>
-  <si>
-    <t>Conoce tu facultad</t>
-  </si>
-  <si>
-    <t>15 min.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horario </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Que el usuario alumno/profesor sea capaz de encontrar su horario de materias inscritas en el cuatimestre actual.  </t>
-  </si>
-  <si>
-    <t>Que el usuario alumno sea capaz de ver y actualizar sus estadisticas de su carrera, las cuales son el porcentaje de la carrera y las materias ya cursadas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Que el usuario pueda encontrar algun salón u edificio de la facultad. </t>
-  </si>
-  <si>
-    <t>Estadística</t>
-  </si>
-  <si>
-    <t>Actualizar estadísticas</t>
-  </si>
-  <si>
-    <t>El usuario alumno proporciona las materias que ya ha cursado, en caso de ser nuevo ingreso no seleccionara nada para el llenado de materias, esto servira para actializar sus estadisticas y que se pueda tener un mejor control de su avance y progreso dentro de la carrera.</t>
-  </si>
-  <si>
-    <t>1 hr.</t>
+    <t xml:space="preserve">Examinar menu de opciones </t>
+  </si>
+  <si>
+    <t>Crea nuevo anuncio</t>
+  </si>
+  <si>
+    <t>Llenar formulario</t>
+  </si>
+  <si>
+    <t>Muestra en la pagina principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Se mostrara un menu en el cual se pueden realizar distintas acciones las cuales se pueden realizar dentro de la plataforma.</t>
+  </si>
+  <si>
+    <t>En esta sección podras realizar un nuevo anunncio para publicar dentro de de la aplicación web.</t>
+  </si>
+  <si>
+    <t>20 min.</t>
+  </si>
+  <si>
+    <t>En esta sección el usuario profesor y unidad academica podran llenar el formulario que corresponde para la publicación del anuncio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iniciar sesión </t>
+  </si>
+  <si>
+    <t>Esta sección se ecnarga del inicio de sesión de usuarios para que se pueda tener acceso y preferencias dependiendo el tipo de usuario.</t>
+  </si>
+  <si>
+    <t>Pagina principal de la aplicación web donde el usuario anonimo puede visualizar los anuncios que existan en la aplicación web.</t>
+  </si>
+  <si>
+    <t>35 min.</t>
   </si>
 </sst>
 </file>
@@ -136,16 +139,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,15 +432,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
@@ -450,115 +456,120 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B20"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>